<commit_message>
before download read the readme
</commit_message>
<xml_diff>
--- a/timetable-double-german.xlsx
+++ b/timetable-double-german.xlsx
@@ -112,37 +112,37 @@
     <t>Politik</t>
   </si>
   <si>
+    <t>Stundenzeiten</t>
+  </si>
+  <si>
+    <t>1.</t>
+  </si>
+  <si>
+    <t>2.</t>
+  </si>
+  <si>
+    <t>3.</t>
+  </si>
+  <si>
+    <t>4.</t>
+  </si>
+  <si>
+    <t>5.</t>
+  </si>
+  <si>
+    <t>6.</t>
+  </si>
+  <si>
+    <t>7.</t>
+  </si>
+  <si>
+    <t>8.</t>
+  </si>
+  <si>
+    <t>Die in dieser Mappe hinzugefügten Fächer / aktualisierten Stundenzeiten werden in der gesamten Arbeitsmappe aktualisiert.</t>
+  </si>
+  <si>
     <t>Fächer</t>
-  </si>
-  <si>
-    <t>Stundenzeiten</t>
-  </si>
-  <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
-    <t>3.</t>
-  </si>
-  <si>
-    <t>4.</t>
-  </si>
-  <si>
-    <t>5.</t>
-  </si>
-  <si>
-    <t>6.</t>
-  </si>
-  <si>
-    <t>7.</t>
-  </si>
-  <si>
-    <t>8.</t>
-  </si>
-  <si>
-    <t>Die in dieser Mappe hinzugefügten Fächer / aktualisierten Stundenzeiten werden in der gesamten Arbeitsmappe aktualisiert.</t>
   </si>
 </sst>
 </file>
@@ -458,6 +458,84 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -470,98 +548,20 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -882,970 +882,982 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="8" width="14.28515625" style="17"/>
-    <col min="9" max="9" width="42.85546875" style="17" customWidth="1"/>
-    <col min="10" max="16384" width="14.28515625" style="17"/>
+    <col min="1" max="8" width="14.28515625" style="7"/>
+    <col min="9" max="9" width="42.85546875" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="14.28515625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:7" hidden="1">
-      <c r="C1" s="17" t="str">
+      <c r="C1" s="7" t="str">
         <f>C35</f>
         <v>Chemie</v>
       </c>
-      <c r="D1" s="17" t="str">
+      <c r="D1" s="7" t="str">
         <f>C1</f>
         <v>Chemie</v>
       </c>
-      <c r="E1" s="17" t="str">
+      <c r="E1" s="7" t="str">
         <f>C1</f>
         <v>Chemie</v>
       </c>
-      <c r="F1" s="17" t="str">
+      <c r="F1" s="7" t="str">
         <f>C1</f>
         <v>Chemie</v>
       </c>
-      <c r="G1" s="17" t="str">
+      <c r="G1" s="7" t="str">
         <f>C1</f>
         <v>Chemie</v>
       </c>
     </row>
     <row r="2" spans="3:7" hidden="1">
-      <c r="C2" s="17" t="str">
+      <c r="C2" s="7" t="str">
         <f>C36</f>
         <v>Deutsch</v>
       </c>
-      <c r="D2" s="17" t="str">
+      <c r="D2" s="7" t="str">
         <f>C2</f>
         <v>Deutsch</v>
       </c>
-      <c r="E2" s="17" t="str">
+      <c r="E2" s="7" t="str">
         <f t="shared" ref="E2:E14" si="0">C2</f>
         <v>Deutsch</v>
       </c>
-      <c r="F2" s="17" t="str">
+      <c r="F2" s="7" t="str">
         <f t="shared" ref="F2:F14" si="1">C2</f>
         <v>Deutsch</v>
       </c>
-      <c r="G2" s="17" t="str">
+      <c r="G2" s="7" t="str">
         <f t="shared" ref="G2:G14" si="2">C2</f>
         <v>Deutsch</v>
       </c>
     </row>
     <row r="3" spans="3:7" hidden="1">
-      <c r="C3" s="17" t="str">
+      <c r="C3" s="7" t="str">
         <f t="shared" ref="C3:C23" si="3">C37</f>
         <v>Englisch</v>
       </c>
-      <c r="D3" s="17" t="str">
+      <c r="D3" s="7" t="str">
         <f t="shared" ref="D3:D23" si="4">C3</f>
         <v>Englisch</v>
       </c>
-      <c r="E3" s="17" t="str">
+      <c r="E3" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Englisch</v>
       </c>
-      <c r="F3" s="17" t="str">
+      <c r="F3" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Englisch</v>
       </c>
-      <c r="G3" s="17" t="str">
+      <c r="G3" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Englisch</v>
       </c>
     </row>
     <row r="4" spans="3:7" hidden="1">
-      <c r="C4" s="17" t="str">
+      <c r="C4" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Erdkunde</v>
       </c>
-      <c r="D4" s="17" t="str">
+      <c r="D4" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Erdkunde</v>
       </c>
-      <c r="E4" s="17" t="str">
+      <c r="E4" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Erdkunde</v>
       </c>
-      <c r="F4" s="17" t="str">
+      <c r="F4" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Erdkunde</v>
       </c>
-      <c r="G4" s="17" t="str">
+      <c r="G4" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Erdkunde</v>
       </c>
     </row>
     <row r="5" spans="3:7" hidden="1">
-      <c r="C5" s="17" t="str">
+      <c r="C5" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Geschichte</v>
       </c>
-      <c r="D5" s="17" t="str">
+      <c r="D5" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Geschichte</v>
       </c>
-      <c r="E5" s="17" t="str">
+      <c r="E5" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Geschichte</v>
       </c>
-      <c r="F5" s="17" t="str">
+      <c r="F5" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Geschichte</v>
       </c>
-      <c r="G5" s="17" t="str">
+      <c r="G5" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Geschichte</v>
       </c>
     </row>
     <row r="6" spans="3:7" hidden="1">
-      <c r="C6" s="17" t="str">
+      <c r="C6" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Kunst</v>
       </c>
-      <c r="D6" s="17" t="str">
+      <c r="D6" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Kunst</v>
       </c>
-      <c r="E6" s="17" t="str">
+      <c r="E6" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Kunst</v>
       </c>
-      <c r="F6" s="17" t="str">
+      <c r="F6" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Kunst</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Kunst</v>
       </c>
     </row>
     <row r="7" spans="3:7" hidden="1">
-      <c r="C7" s="17" t="str">
+      <c r="C7" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Latein</v>
       </c>
-      <c r="D7" s="17" t="str">
+      <c r="D7" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Latein</v>
       </c>
-      <c r="E7" s="17" t="str">
+      <c r="E7" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Latein</v>
       </c>
-      <c r="F7" s="17" t="str">
+      <c r="F7" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Latein</v>
       </c>
-      <c r="G7" s="17" t="str">
+      <c r="G7" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Latein</v>
       </c>
     </row>
     <row r="8" spans="3:7" hidden="1">
-      <c r="C8" s="17" t="str">
+      <c r="C8" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Mathe</v>
       </c>
-      <c r="D8" s="17" t="str">
+      <c r="D8" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Mathe</v>
       </c>
-      <c r="E8" s="17" t="str">
+      <c r="E8" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Mathe</v>
       </c>
-      <c r="F8" s="17" t="str">
+      <c r="F8" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Mathe</v>
       </c>
-      <c r="G8" s="17" t="str">
+      <c r="G8" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Mathe</v>
       </c>
     </row>
     <row r="9" spans="3:7" hidden="1">
-      <c r="C9" s="17" t="str">
+      <c r="C9" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Musik</v>
       </c>
-      <c r="D9" s="17" t="str">
+      <c r="D9" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Musik</v>
       </c>
-      <c r="E9" s="17" t="str">
+      <c r="E9" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Musik</v>
       </c>
-      <c r="F9" s="17" t="str">
+      <c r="F9" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Musik</v>
       </c>
-      <c r="G9" s="17" t="str">
+      <c r="G9" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Musik</v>
       </c>
     </row>
     <row r="10" spans="3:7" hidden="1">
-      <c r="C10" s="17" t="str">
+      <c r="C10" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Physik</v>
       </c>
-      <c r="D10" s="17" t="str">
+      <c r="D10" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Physik</v>
       </c>
-      <c r="E10" s="17" t="str">
+      <c r="E10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Physik</v>
       </c>
-      <c r="F10" s="17" t="str">
+      <c r="F10" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Physik</v>
       </c>
-      <c r="G10" s="17" t="str">
+      <c r="G10" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Physik</v>
       </c>
     </row>
     <row r="11" spans="3:7" hidden="1">
-      <c r="C11" s="17" t="str">
+      <c r="C11" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Politik</v>
       </c>
-      <c r="D11" s="17" t="str">
+      <c r="D11" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Politik</v>
       </c>
-      <c r="E11" s="17" t="str">
+      <c r="E11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Politik</v>
       </c>
-      <c r="F11" s="17" t="str">
+      <c r="F11" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Politik</v>
       </c>
-      <c r="G11" s="17" t="str">
+      <c r="G11" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Politik</v>
       </c>
     </row>
     <row r="12" spans="3:7" hidden="1">
-      <c r="C12" s="17" t="str">
+      <c r="C12" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Religion</v>
       </c>
-      <c r="D12" s="17" t="str">
+      <c r="D12" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Religion</v>
       </c>
-      <c r="E12" s="17" t="str">
+      <c r="E12" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Religion</v>
       </c>
-      <c r="F12" s="17" t="str">
+      <c r="F12" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Religion</v>
       </c>
-      <c r="G12" s="17" t="str">
+      <c r="G12" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Religion</v>
       </c>
     </row>
     <row r="13" spans="3:7" hidden="1">
-      <c r="C13" s="17" t="str">
+      <c r="C13" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Sport</v>
       </c>
-      <c r="D13" s="17" t="str">
+      <c r="D13" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Sport</v>
       </c>
-      <c r="E13" s="17" t="str">
+      <c r="E13" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Sport</v>
       </c>
-      <c r="F13" s="17" t="str">
+      <c r="F13" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Sport</v>
       </c>
-      <c r="G13" s="17" t="str">
+      <c r="G13" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Sport</v>
       </c>
     </row>
     <row r="14" spans="3:7" hidden="1">
-      <c r="C14" s="17" t="str">
+      <c r="C14" s="7" t="str">
         <f t="shared" si="3"/>
         <v>Schwimmen</v>
       </c>
-      <c r="D14" s="17" t="str">
+      <c r="D14" s="7" t="str">
         <f t="shared" si="4"/>
         <v>Schwimmen</v>
       </c>
-      <c r="E14" s="17" t="str">
+      <c r="E14" s="7" t="str">
         <f t="shared" si="0"/>
         <v>Schwimmen</v>
       </c>
-      <c r="F14" s="17" t="str">
+      <c r="F14" s="7" t="str">
         <f t="shared" si="1"/>
         <v>Schwimmen</v>
       </c>
-      <c r="G14" s="17" t="str">
+      <c r="G14" s="7" t="str">
         <f t="shared" si="2"/>
         <v>Schwimmen</v>
       </c>
     </row>
     <row r="15" spans="3:7" hidden="1">
-      <c r="C15" s="17">
+      <c r="C15" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="7">
         <f t="shared" ref="E15:E23" si="5">C15</f>
         <v>0</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="7">
         <f t="shared" ref="F15:F23" si="6">C15</f>
         <v>0</v>
       </c>
-      <c r="G15" s="17">
+      <c r="G15" s="7">
         <f t="shared" ref="G15:G23" si="7">C15</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="3:7" hidden="1">
-      <c r="C16" s="17">
+      <c r="C16" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G16" s="17">
+      <c r="G16" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:10" hidden="1">
-      <c r="C17" s="17">
+      <c r="C17" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G17" s="17">
+      <c r="G17" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:10" hidden="1">
-      <c r="C18" s="17">
+      <c r="C18" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G18" s="17">
+      <c r="G18" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:10" hidden="1">
-      <c r="C19" s="17">
+      <c r="C19" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G19" s="17">
+      <c r="G19" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:10" hidden="1">
-      <c r="C20" s="17">
+      <c r="C20" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:10" hidden="1">
-      <c r="C21" s="17">
+      <c r="C21" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G21" s="17">
+      <c r="G21" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:10" hidden="1">
-      <c r="C22" s="17">
+      <c r="C22" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G22" s="17">
+      <c r="G22" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15.75" hidden="1" thickBot="1">
-      <c r="C23" s="17">
+      <c r="C23" s="7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="7">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="7">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G23" s="17">
+      <c r="G23" s="7">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="23.25" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A24" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24" s="18" t="s">
+      <c r="A24" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="18" t="s">
+      <c r="E24" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="I24" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="J24" s="19"/>
+      <c r="J24" s="31"/>
     </row>
     <row r="25" spans="1:10" ht="23.25" hidden="1" customHeight="1" thickTop="1">
-      <c r="A25" s="20">
+      <c r="A25" s="9">
         <v>1</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="6"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:10" ht="23.25" hidden="1" customHeight="1" thickBot="1">
-      <c r="A26" s="21">
+      <c r="A26" s="10">
         <v>2</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="7"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:10" ht="30.75" hidden="1" thickTop="1">
-      <c r="A27" s="20">
+      <c r="A27" s="9">
         <v>3</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="30.75" hidden="1" thickBot="1">
-      <c r="A28" s="21">
+      <c r="A28" s="10">
         <v>4</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="1:10" ht="30.75" hidden="1" thickTop="1">
-      <c r="A29" s="20">
+      <c r="A29" s="9">
         <v>5</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
-      <c r="J29" s="22"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10" ht="23.25" hidden="1" customHeight="1" thickBot="1">
-      <c r="A30" s="21">
+      <c r="A30" s="10">
         <v>6</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="23.25" hidden="1" customHeight="1" thickTop="1">
-      <c r="A31" s="20">
+      <c r="A31" s="9">
         <v>7</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:10" ht="30.75" hidden="1" thickBot="1">
-      <c r="A32" s="21">
+      <c r="A32" s="10">
         <v>8</v>
       </c>
-      <c r="B32" s="21" t="s">
+      <c r="B32" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="1:15" ht="23.25" hidden="1" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B33" s="23"/>
+      <c r="B33" s="12"/>
     </row>
     <row r="34" spans="1:15" ht="30" customHeight="1" thickBot="1">
-      <c r="B34" s="24"/>
-      <c r="C34" s="12" t="s">
+      <c r="B34" s="13"/>
+      <c r="C34" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="40"/>
+      <c r="H34" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="13"/>
-      <c r="H34" s="14" t="s">
+      <c r="I34" s="25"/>
+      <c r="J34" s="11"/>
+    </row>
+    <row r="35" spans="1:15" ht="22.5" customHeight="1">
+      <c r="A35" s="11"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="30"/>
+      <c r="H35" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I34" s="15"/>
-      <c r="J34" s="22"/>
-    </row>
-    <row r="35" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A35" s="22"/>
-      <c r="B35" s="25"/>
-      <c r="C35" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="28"/>
-      <c r="H35" s="29" t="s">
+      <c r="I35" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="11"/>
+    </row>
+    <row r="36" spans="1:15" ht="22.5" customHeight="1">
+      <c r="A36" s="11"/>
+      <c r="B36" s="14"/>
+      <c r="C36" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
+      <c r="H36" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="I35" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="J35" s="22"/>
-    </row>
-    <row r="36" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A36" s="22"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" s="27"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="28"/>
-      <c r="H36" s="31" t="s">
+      <c r="I36" s="18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" ht="22.5" customHeight="1">
+      <c r="B37" s="14"/>
+      <c r="C37" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="30"/>
+      <c r="H37" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I36" s="32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" ht="22.5" customHeight="1">
-      <c r="B37" s="25"/>
-      <c r="C37" s="26" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="27"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="28"/>
-      <c r="H37" s="31" t="s">
+      <c r="I37" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" ht="22.5" customHeight="1">
+      <c r="A38" s="11"/>
+      <c r="B38" s="14"/>
+      <c r="C38" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="30"/>
+      <c r="H38" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="I37" s="33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A38" s="22"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="28"/>
-      <c r="H38" s="31" t="s">
+      <c r="I38" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="22.5" customHeight="1">
+      <c r="A39" s="11"/>
+      <c r="B39" s="14"/>
+      <c r="C39" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="30"/>
+      <c r="H39" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="I38" s="32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A39" s="22"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="28"/>
-      <c r="H39" s="31" t="s">
+      <c r="I39" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="22.5" customHeight="1">
+      <c r="A40" s="11"/>
+      <c r="B40" s="14"/>
+      <c r="C40" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="30"/>
+      <c r="H40" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="I39" s="33" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A40" s="22"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="28"/>
-      <c r="H40" s="31" t="s">
+      <c r="I40" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" ht="22.5" customHeight="1">
+      <c r="A41" s="11"/>
+      <c r="B41" s="14"/>
+      <c r="C41" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="30"/>
+      <c r="H41" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="I40" s="32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A41" s="22"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="28"/>
-      <c r="H41" s="31" t="s">
+      <c r="I41" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" ht="22.5" customHeight="1" thickBot="1">
+      <c r="A42" s="11"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="30"/>
+      <c r="H42" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="I41" s="33" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A42" s="22"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="28"/>
-      <c r="H42" s="34" t="s">
+      <c r="I42" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" ht="22.5" customHeight="1">
+      <c r="A43" s="11"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="30"/>
+      <c r="N43" s="22"/>
+      <c r="O43" s="22"/>
+    </row>
+    <row r="44" spans="1:15" ht="22.5" customHeight="1">
+      <c r="A44" s="11"/>
+      <c r="B44" s="14"/>
+      <c r="C44" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="30"/>
+      <c r="H44" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="I42" s="35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A43" s="22"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="28"/>
-      <c r="N43" s="36"/>
-      <c r="O43" s="36"/>
-    </row>
-    <row r="44" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A44" s="22"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="28"/>
-      <c r="H44" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="N44" s="36"/>
-      <c r="O44" s="36"/>
+      <c r="N44" s="22"/>
+      <c r="O44" s="22"/>
     </row>
     <row r="45" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A45" s="22"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="26" t="s">
+      <c r="A45" s="11"/>
+      <c r="B45" s="14"/>
+      <c r="C45" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="28"/>
-      <c r="N45" s="36"/>
-      <c r="O45" s="36"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="30"/>
+      <c r="N45" s="22"/>
+      <c r="O45" s="22"/>
     </row>
     <row r="46" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A46" s="22"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="26" t="s">
+      <c r="A46" s="11"/>
+      <c r="B46" s="14"/>
+      <c r="C46" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="28"/>
-      <c r="N46" s="36"/>
-      <c r="O46" s="36"/>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="30"/>
+      <c r="N46" s="22"/>
+      <c r="O46" s="22"/>
     </row>
     <row r="47" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A47" s="22"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="26" t="s">
+      <c r="A47" s="11"/>
+      <c r="B47" s="14"/>
+      <c r="C47" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="28"/>
-      <c r="N47" s="36"/>
-      <c r="O47" s="36"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="30"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
     </row>
     <row r="48" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A48" s="22"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="26" t="s">
+      <c r="A48" s="11"/>
+      <c r="B48" s="14"/>
+      <c r="C48" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="28"/>
-      <c r="N48" s="36"/>
-      <c r="O48" s="36"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="30"/>
+      <c r="N48" s="22"/>
+      <c r="O48" s="22"/>
     </row>
     <row r="49" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A49" s="22"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="28"/>
-      <c r="N49" s="36"/>
-      <c r="O49" s="36"/>
+      <c r="A49" s="11"/>
+      <c r="B49" s="14"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="30"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="22"/>
     </row>
     <row r="50" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A50" s="22"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="28"/>
-      <c r="N50" s="36"/>
-      <c r="O50" s="36"/>
+      <c r="A50" s="11"/>
+      <c r="B50" s="14"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="30"/>
+      <c r="N50" s="22"/>
+      <c r="O50" s="22"/>
     </row>
     <row r="51" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A51" s="22"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="26"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="28"/>
-      <c r="N51" s="36"/>
-      <c r="O51" s="36"/>
+      <c r="A51" s="11"/>
+      <c r="B51" s="14"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="30"/>
+      <c r="N51" s="22"/>
+      <c r="O51" s="22"/>
     </row>
     <row r="52" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A52" s="22"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="28"/>
-      <c r="N52" s="36"/>
-      <c r="O52" s="36"/>
+      <c r="A52" s="11"/>
+      <c r="B52" s="14"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29"/>
+      <c r="F52" s="30"/>
+      <c r="N52" s="22"/>
+      <c r="O52" s="22"/>
     </row>
     <row r="53" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A53" s="22"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="26"/>
-      <c r="D53" s="27"/>
-      <c r="E53" s="27"/>
-      <c r="F53" s="28"/>
-      <c r="N53" s="36"/>
-      <c r="O53" s="36"/>
+      <c r="A53" s="11"/>
+      <c r="B53" s="14"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="30"/>
+      <c r="N53" s="22"/>
+      <c r="O53" s="22"/>
     </row>
     <row r="54" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A54" s="22"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="28"/>
-      <c r="N54" s="36"/>
-      <c r="O54" s="36"/>
+      <c r="A54" s="11"/>
+      <c r="B54" s="14"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="30"/>
+      <c r="N54" s="22"/>
+      <c r="O54" s="22"/>
     </row>
     <row r="55" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A55" s="22"/>
-      <c r="B55" s="25"/>
-      <c r="C55" s="26"/>
-      <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
-      <c r="F55" s="28"/>
-      <c r="N55" s="36"/>
-      <c r="O55" s="36"/>
+      <c r="A55" s="11"/>
+      <c r="B55" s="14"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="29"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="30"/>
+      <c r="N55" s="22"/>
+      <c r="O55" s="22"/>
     </row>
     <row r="56" spans="1:15" ht="22.5" customHeight="1">
-      <c r="A56" s="22"/>
-      <c r="B56" s="25"/>
-      <c r="C56" s="26"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="28"/>
-      <c r="N56" s="36"/>
-      <c r="O56" s="36"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="14"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="30"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="22"/>
     </row>
     <row r="57" spans="1:15" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A57" s="22"/>
-      <c r="B57" s="25"/>
-      <c r="C57" s="38"/>
-      <c r="D57" s="39"/>
-      <c r="E57" s="39"/>
-      <c r="F57" s="40"/>
-      <c r="N57" s="36"/>
-      <c r="O57" s="36"/>
+      <c r="A57" s="11"/>
+      <c r="B57" s="14"/>
+      <c r="C57" s="36"/>
+      <c r="D57" s="37"/>
+      <c r="E57" s="37"/>
+      <c r="F57" s="38"/>
+      <c r="N57" s="22"/>
+      <c r="O57" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="G31:G32"/>
+    <mergeCell ref="C54:F54"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="C56:F56"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C35:F35"/>
+    <mergeCell ref="C36:F36"/>
+    <mergeCell ref="C37:F37"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="C42:F42"/>
+    <mergeCell ref="C43:F43"/>
+    <mergeCell ref="C44:F44"/>
+    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C50:F50"/>
+    <mergeCell ref="C51:F51"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="C53:F53"/>
     <mergeCell ref="C46:F46"/>
     <mergeCell ref="C47:F47"/>
     <mergeCell ref="C48:F48"/>
@@ -1862,27 +1874,15 @@
     <mergeCell ref="G29:G30"/>
     <mergeCell ref="C27:C28"/>
     <mergeCell ref="D27:D28"/>
-    <mergeCell ref="C49:F49"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="C51:F51"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="C54:F54"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="C56:F56"/>
-    <mergeCell ref="C57:F57"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C35:F35"/>
-    <mergeCell ref="C36:F36"/>
-    <mergeCell ref="C37:F37"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="C42:F42"/>
-    <mergeCell ref="C43:F43"/>
-    <mergeCell ref="C44:F44"/>
-    <mergeCell ref="C45:F45"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="G31:G32"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C25:G32">
@@ -2458,25 +2458,25 @@
         <f>Vorlage!I35</f>
         <v xml:space="preserve">  7.50-  8.35 Uhr</v>
       </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="6"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:10" ht="16.5" customHeight="1" thickBot="1">
       <c r="A26" s="3">
         <v>2</v>
       </c>
-      <c r="B26" s="16" t="str">
+      <c r="B26" s="6" t="str">
         <f>Vorlage!I36</f>
         <v xml:space="preserve">  8.40-  9.25 Uhr</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="7"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="33"/>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickTop="1">
       <c r="A27" s="4">
@@ -2486,25 +2486,25 @@
         <f>Vorlage!I37</f>
         <v xml:space="preserve">  9.45-10.30 Uhr</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1">
       <c r="A28" s="3">
         <v>4</v>
       </c>
-      <c r="B28" s="16" t="str">
+      <c r="B28" s="6" t="str">
         <f>Vorlage!I38</f>
         <v>10. 35-11.20 Uhr</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
     </row>
     <row r="29" spans="1:10" ht="15.75" thickTop="1">
       <c r="A29" s="4">
@@ -2514,26 +2514,26 @@
         <f>Vorlage!I39</f>
         <v>11.35-12.20 Uhr</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
       <c r="J29" s="1"/>
     </row>
     <row r="30" spans="1:10" ht="16.5" customHeight="1" thickBot="1">
       <c r="A30" s="3">
         <v>6</v>
       </c>
-      <c r="B30" s="16" t="str">
+      <c r="B30" s="6" t="str">
         <f>Vorlage!I40</f>
         <v>12.25-13.10 Uhr</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" thickTop="1">
       <c r="A31" s="4">
@@ -2543,11 +2543,11 @@
         <f>Vorlage!I41</f>
         <v>13.50-14.35 Uhr</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
     </row>
     <row r="32" spans="1:10" ht="15.75" thickBot="1">
       <c r="A32" s="3">
@@ -2557,11 +2557,11 @@
         <f>Vorlage!I42</f>
         <v>14.40-15.20 Uhr</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
     </row>
     <row r="33" spans="10:10" ht="16.5" customHeight="1" thickTop="1"/>
     <row r="34" spans="10:10">
@@ -2572,26 +2572,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="G25:G26"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
     <mergeCell ref="C31:C32"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="G31:G32"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="G25:G26"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Falsches Fach" error="Du hast dieses Fach noch nicht hinzugefügt!_x000a_Weitere Informationen zum Hinzufügen von Fächern unter silas229.pe.hu/more/" sqref="D25:G32 C27:C32">

</xml_diff>